<commit_message>
May 28 2020 update
</commit_message>
<xml_diff>
--- a/Output/Tables/Table_1.xlsx
+++ b/Output/Tables/Table_1.xlsx
@@ -170,13 +170,13 @@
         <v>7.3690271E7</v>
       </c>
       <c r="E3" t="n">
-        <v>747437.0169520816</v>
+        <v>915763.7357711862</v>
       </c>
       <c r="F3" t="n">
-        <v>131739.18494582784</v>
+        <v>163505.01289087508</v>
       </c>
       <c r="G3" t="n">
-        <v>17.6</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="4">
@@ -193,13 +193,13 @@
         <v>1.3763183E7</v>
       </c>
       <c r="E4" t="n">
-        <v>140799.44976942134</v>
+        <v>171037.82777760012</v>
       </c>
       <c r="F4" t="n">
-        <v>13788.245481967964</v>
+        <v>16664.416194232548</v>
       </c>
       <c r="G4" t="n">
-        <v>9.8</v>
+        <v>9.7</v>
       </c>
     </row>
     <row r="5">
@@ -216,13 +216,13 @@
         <v>6994464.0</v>
       </c>
       <c r="E5" t="n">
-        <v>70524.4283328685</v>
+        <v>86921.60302080003</v>
       </c>
       <c r="F5" t="n">
-        <v>9206.253918067034</v>
+        <v>11340.8056353941</v>
       </c>
       <c r="G5" t="n">
-        <v>13.1</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="6">
@@ -239,13 +239,13 @@
         <v>5.2932624E7</v>
       </c>
       <c r="E6" t="n">
-        <v>536113.1388497888</v>
+        <v>657804.3049727976</v>
       </c>
       <c r="F6" t="n">
-        <v>108744.68554579285</v>
+        <v>135499.7910612484</v>
       </c>
       <c r="G6" t="n">
-        <v>20.3</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="7">
@@ -262,13 +262,13 @@
         <v>1.2770843E7</v>
       </c>
       <c r="E7" t="n">
-        <v>132842.72648362408</v>
+        <v>158705.82012960006</v>
       </c>
       <c r="F7" t="n">
-        <v>24698.685914210517</v>
+        <v>29714.801234687355</v>
       </c>
       <c r="G7" t="n">
-        <v>18.6</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="8">
@@ -285,13 +285,13 @@
         <v>1.8573954E7</v>
       </c>
       <c r="E8" t="n">
-        <v>188466.4633391537</v>
+        <v>230822.24114880018</v>
       </c>
       <c r="F8" t="n">
-        <v>32088.356022378066</v>
+        <v>39800.924230264754</v>
       </c>
       <c r="G8" t="n">
-        <v>17.0</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="9">
@@ -308,13 +308,13 @@
         <v>2.1953876E7</v>
       </c>
       <c r="E9" t="n">
-        <v>221333.65563514622</v>
+        <v>272825.2078272002</v>
       </c>
       <c r="F9" t="n">
-        <v>37253.164813296265</v>
+        <v>46702.59660070997</v>
       </c>
       <c r="G9" t="n">
-        <v>16.8</v>
+        <v>17.1</v>
       </c>
     </row>
     <row r="10">
@@ -331,13 +331,13 @@
         <v>2614804.0</v>
       </c>
       <c r="E10" t="n">
-        <v>27769.66793988588</v>
+        <v>32494.692268800005</v>
       </c>
       <c r="F10" t="n">
-        <v>5786.323580669973</v>
+        <v>6787.807567225531</v>
       </c>
       <c r="G10" t="n">
-        <v>20.8</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="11">
@@ -354,13 +354,13 @@
         <v>1.7763239E7</v>
       </c>
       <c r="E11" t="n">
-        <v>176880.05458499413</v>
+        <v>220747.3237008001</v>
       </c>
       <c r="F11" t="n">
-        <v>31885.288370645212</v>
+        <v>40466.90267813935</v>
       </c>
       <c r="G11" t="n">
-        <v>18.0</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="12">
@@ -377,13 +377,13 @@
         <v>13555.0</v>
       </c>
       <c r="E12" t="n">
-        <v>144.44896927485271</v>
+        <v>168.450696</v>
       </c>
       <c r="F12" t="n">
-        <v>27.366244627812236</v>
+        <v>31.98057984809888</v>
       </c>
       <c r="G12" t="n">
-        <v>18.9</v>
+        <v>19.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates the asthma_rate.RDS to include national average rates instead of random error meta
</commit_message>
<xml_diff>
--- a/Output/Tables/Table_1.xlsx
+++ b/Output/Tables/Table_1.xlsx
@@ -170,13 +170,13 @@
         <v>7.3690271E7</v>
       </c>
       <c r="E3" t="n">
-        <v>915763.7357711862</v>
+        <v>679025.8923849599</v>
       </c>
       <c r="F3" t="n">
-        <v>163505.01289087508</v>
+        <v>138914.46882130537</v>
       </c>
       <c r="G3" t="n">
-        <v>17.9</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="4">
@@ -193,13 +193,13 @@
         <v>1.3763183E7</v>
       </c>
       <c r="E4" t="n">
-        <v>171037.82777760012</v>
+        <v>126789.67668903836</v>
       </c>
       <c r="F4" t="n">
-        <v>16664.416194232548</v>
+        <v>14516.597729148474</v>
       </c>
       <c r="G4" t="n">
-        <v>9.7</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="5">
@@ -216,13 +216,13 @@
         <v>6994464.0</v>
       </c>
       <c r="E5" t="n">
-        <v>86921.60302080003</v>
+        <v>64519.75085621432</v>
       </c>
       <c r="F5" t="n">
-        <v>11340.8056353941</v>
+        <v>9845.141984185488</v>
       </c>
       <c r="G5" t="n">
-        <v>13.0</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="6">
@@ -239,13 +239,13 @@
         <v>5.2932624E7</v>
       </c>
       <c r="E6" t="n">
-        <v>657804.3049727976</v>
+        <v>487716.46483970823</v>
       </c>
       <c r="F6" t="n">
-        <v>135499.7910612484</v>
+        <v>114552.72910797142</v>
       </c>
       <c r="G6" t="n">
-        <v>20.6</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="7">
@@ -262,13 +262,13 @@
         <v>1.2770843E7</v>
       </c>
       <c r="E7" t="n">
-        <v>158705.82012960006</v>
+        <v>121243.75723927609</v>
       </c>
       <c r="F7" t="n">
-        <v>29714.801234687355</v>
+        <v>26125.173186287033</v>
       </c>
       <c r="G7" t="n">
-        <v>18.7</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="8">
@@ -285,13 +285,13 @@
         <v>1.8573954E7</v>
       </c>
       <c r="E8" t="n">
-        <v>230822.24114880018</v>
+        <v>171097.71222410485</v>
       </c>
       <c r="F8" t="n">
-        <v>39800.924230264754</v>
+        <v>33849.03757102444</v>
       </c>
       <c r="G8" t="n">
-        <v>17.2</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="9">
@@ -308,13 +308,13 @@
         <v>2.1953876E7</v>
       </c>
       <c r="E9" t="n">
-        <v>272825.2078272002</v>
+        <v>200942.87287758396</v>
       </c>
       <c r="F9" t="n">
-        <v>46702.59660070997</v>
+        <v>39263.165425997526</v>
       </c>
       <c r="G9" t="n">
-        <v>17.1</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="10">
@@ -331,13 +331,13 @@
         <v>2614804.0</v>
       </c>
       <c r="E10" t="n">
-        <v>32494.692268800005</v>
+        <v>25238.457391499036</v>
       </c>
       <c r="F10" t="n">
-        <v>6787.807567225531</v>
+        <v>6052.406386566344</v>
       </c>
       <c r="G10" t="n">
-        <v>20.9</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="11">
@@ -354,13 +354,13 @@
         <v>1.7763239E7</v>
       </c>
       <c r="E11" t="n">
-        <v>220747.3237008001</v>
+        <v>160372.4625551049</v>
       </c>
       <c r="F11" t="n">
-        <v>40466.90267813935</v>
+        <v>33595.9699673872</v>
       </c>
       <c r="G11" t="n">
-        <v>18.3</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="12">
@@ -377,13 +377,13 @@
         <v>13555.0</v>
       </c>
       <c r="E12" t="n">
-        <v>168.450696</v>
+        <v>130.6300973915227</v>
       </c>
       <c r="F12" t="n">
-        <v>31.98057984809888</v>
+        <v>28.716284042823688</v>
       </c>
       <c r="G12" t="n">
-        <v>19.0</v>
+        <v>22.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>